<commit_message>
Further work on SVM
</commit_message>
<xml_diff>
--- a/Dataset/Dataset.xlsx
+++ b/Dataset/Dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Filippo\Documents\Proj inz\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A0B3B1E-0CD9-41FC-9E83-7462BE8FE142}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ECD8088-587F-4DEE-825D-3657007B1128}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-2190" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -2050,16 +2050,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2086,16 +2086,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2388,8 +2388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>